<commit_message>
added changings in write cast logic
</commit_message>
<xml_diff>
--- a/target/test-classes/qaautomationdata.xlsx
+++ b/target/test-classes/qaautomationdata.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>Series Cast</t>
   </si>
@@ -108,22 +108,10 @@
     <t>GET</t>
   </si>
   <si>
-    <t>Expected Response Code</t>
-  </si>
-  <si>
-    <t>Expected Response time in seconds (less than)</t>
-  </si>
-  <si>
-    <t>Expected Response Size in kilobyte (less than)</t>
-  </si>
-  <si>
     <t>https://emumba-test.herokuapp.com/user</t>
   </si>
   <si>
     <t>POST</t>
-  </si>
-  <si>
-    <t>Request Payload (json)</t>
   </si>
   <si>
     <t>N/A</t>
@@ -156,9 +144,6 @@
     <t>"email", "first_name", "last_name", "plan", "id", "access_token", "refresh_token"</t>
   </si>
   <si>
-    <t>Condititions/Assertions</t>
-  </si>
-  <si>
     <t>firstName</t>
   </si>
   <si>
@@ -202,13 +187,25 @@
   </si>
   <si>
     <t>after life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request Payload </t>
+  </si>
+  <si>
+    <t>Response Size</t>
+  </si>
+  <si>
+    <t>Response time</t>
+  </si>
+  <si>
+    <t>Response Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,12 +236,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -265,14 +256,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -300,33 +283,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -627,12 +604,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -643,73 +620,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="49.5546875" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-    </row>
-    <row r="2" spans="1:8" ht="109.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="31.3" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="66.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="4">
+        <v>201</v>
+      </c>
+      <c r="F2" s="4">
+        <v>1</v>
+      </c>
+      <c r="G2" s="4">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="105.65" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="66.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -719,52 +709,38 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="105.65" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="92.35" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="E4" s="4">
         <v>200</v>
       </c>
       <c r="F4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4" s="4">
         <v>2</v>
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="92.35" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="4">
-        <v>200</v>
-      </c>
-      <c r="F5" s="4">
-        <v>2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>2</v>
-      </c>
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
@@ -807,23 +783,10 @@
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:G1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -846,11 +809,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1084,71 +1047,71 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
-      </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>1231233</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E3">
         <v>2342344</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>